<commit_message>
added some tables with descriptive statistics
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EduScience\Articles\Core_RISC_2022_2023\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\EduScience\Articles\Core_RISC_2022_2023\repo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C1E39A-F4D9-4B34-A67D-D82E262F7B5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94A22BA4-57F4-40BB-B25D-9168CAF4AFD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{C74EF8FA-AD40-45EA-A7D2-8F8839E2C7A5}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="135">
   <si>
     <t>Всего</t>
   </si>
@@ -1324,6 +1324,192 @@
     </r>
   </si>
   <si>
+    <t>X50</t>
+  </si>
+  <si>
+    <t>X51</t>
+  </si>
+  <si>
+    <t>X46</t>
+  </si>
+  <si>
+    <t>X47</t>
+  </si>
+  <si>
+    <t>X48</t>
+  </si>
+  <si>
+    <t>X49</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">X46 - Цели использования веб-сайта </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>всего</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, в процентах от общего числа организаций</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">X47 - Цели использования веб-сайта </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>публикации каталогов товаров  (работ, услуг) или прейскурантов</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, в процентах от общего числа организаций</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">X48 - Цели использования веб-сайта </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>публикации вакансий на рабочие места или приема онлайн- заявлений на работу</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, в процентах от общего числа организаций</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">X49 - Цели использования веб-сайта </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>размещения версии веб-сайта для пользователей мобильной связи</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, в процентах от общего числа организаций</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">X50 - Цели использования веб-сайта </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>онлайновой системы платежей</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, в процентах от общего числа организаций</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">X51 - Цели использования веб-сайта </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>отслеживания статуса заказов</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>, в процентах от общего числа организаций</t>
+    </r>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">X39 - Общие цели использования сети Интернет </t>
     </r>
@@ -1337,7 +1523,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>Профессиональная подготовка персонала</t>
+      <t>Подписка на доступ к электронным базам данных, электронным библиотекам на платной основе</t>
     </r>
     <r>
       <rPr>
@@ -1353,7 +1539,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">X40 - Коммерческие цели использования сети Интернет </t>
+      <t xml:space="preserve">X40 - Коммерческие цели использования сети Интернет для связи с потребителями </t>
     </r>
     <r>
       <rPr>
@@ -1381,7 +1567,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">X41 - Коммерческие цели использования сети Интернет </t>
+      <t xml:space="preserve">X41 - Коммерческие цели использования сети Интернет для связи с потребителями </t>
     </r>
     <r>
       <rPr>
@@ -1409,7 +1595,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">X42 - Коммерческие цели использования сети Интернет </t>
+      <t xml:space="preserve">X42 - Коммерческие цели использования сети Интернет для связи с потребителями </t>
     </r>
     <r>
       <rPr>
@@ -1437,7 +1623,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">X43 - Коммерческие цели использования сети Интернет </t>
+      <t xml:space="preserve">X43 - Коммерческие цели использования сети Интернет для связи с потребителями </t>
     </r>
     <r>
       <rPr>
@@ -1449,7 +1635,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>на выпускаемые организацией товары (работы, услуги) (без учета заказов, отправленных по электронной почте)</t>
+      <t>получение заказов на выпускаемые организацией товары (работы, услуги) (без учета заказов, отправленных по электронной почте)</t>
     </r>
     <r>
       <rPr>
@@ -1465,7 +1651,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">X44 - Коммерческие цели использования сети Интернет </t>
+      <t xml:space="preserve">X44 - Коммерческие цели использования сети Интернет для связи с потребителями  </t>
     </r>
     <r>
       <rPr>
@@ -1493,7 +1679,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">X45 - Коммерческие цели использования сети Интернет </t>
+      <t xml:space="preserve">X45 - Коммерческие цели использования сети Интернет для связи с потребителями </t>
     </r>
     <r>
       <rPr>
@@ -1520,26 +1706,8 @@
     </r>
   </si>
   <si>
-    <t>X50</t>
-  </si>
-  <si>
-    <t>X51</t>
-  </si>
-  <si>
-    <t>X46</t>
-  </si>
-  <si>
-    <t>X47</t>
-  </si>
-  <si>
-    <t>X48</t>
-  </si>
-  <si>
-    <t>X49</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">X46 - Цели использования веб-сайта </t>
+    <r>
+      <t xml:space="preserve">X52 -  Коммерческие цели использования сети Интернет для связи с поставщиками </t>
     </r>
     <r>
       <rPr>
@@ -1567,7 +1735,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">X47 - Цели использования веб-сайта </t>
+      <t xml:space="preserve">X53 -  Коммерческие цели использования сети Интернет для связи с поставщиками </t>
     </r>
     <r>
       <rPr>
@@ -1579,7 +1747,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>публикации каталогов товаров  (работ, услуг) или прейскурантов</t>
+      <t>получение сведений о необходимых товарах (работах, услугах) и их поставщиках</t>
     </r>
     <r>
       <rPr>
@@ -1595,7 +1763,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">X48 - Цели использования веб-сайта </t>
+      <t xml:space="preserve">X54 -  Коммерческие цели использования сети Интернет для связи с поставщиками </t>
     </r>
     <r>
       <rPr>
@@ -1607,7 +1775,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>публикации вакансий на рабочие места или приема онлайн- заявлений на работу</t>
+      <t>предоставление сведений о потребностях организации в товарах (работах, услугах)</t>
     </r>
     <r>
       <rPr>
@@ -1623,7 +1791,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">X49 - Цели использования веб-сайта </t>
+      <t xml:space="preserve">X55 -  Коммерческие цели использования сети Интернет для связи с поставщиками </t>
     </r>
     <r>
       <rPr>
@@ -1635,7 +1803,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>размещения версии веб-сайта для пользователей мобильной связи</t>
+      <t>оплата поставляемых товаров (работ, услуг)</t>
     </r>
     <r>
       <rPr>
@@ -1651,7 +1819,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">X50 - Цели использования веб-сайта </t>
+      <t xml:space="preserve">X56 -  Коммерческие цели использования сети Интернет для связи с поставщиками </t>
     </r>
     <r>
       <rPr>
@@ -1663,7 +1831,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>онлайновой системы платежей</t>
+      <t>размещение заказов на необходимые организации  товары (работы, услуги) (без учета заказов, отправленных по электронной почте)</t>
     </r>
     <r>
       <rPr>
@@ -1679,7 +1847,7 @@
   </si>
   <si>
     <r>
-      <t xml:space="preserve">X51 - Цели использования веб-сайта </t>
+      <t xml:space="preserve">X57 -  Коммерческие цели использования сети Интернет для связи с поставщиками </t>
     </r>
     <r>
       <rPr>
@@ -1691,7 +1859,7 @@
         <charset val="204"/>
         <scheme val="minor"/>
       </rPr>
-      <t>отслеживания статуса заказов</t>
+      <t>получение электронной продукции</t>
     </r>
     <r>
       <rPr>
@@ -1704,6 +1872,24 @@
       </rPr>
       <t>, в процентах от общего числа организаций</t>
     </r>
+  </si>
+  <si>
+    <t>X52</t>
+  </si>
+  <si>
+    <t>X53</t>
+  </si>
+  <si>
+    <t>X54</t>
+  </si>
+  <si>
+    <t>X55</t>
+  </si>
+  <si>
+    <t>X56</t>
+  </si>
+  <si>
+    <t>X57</t>
   </si>
 </sst>
 </file>
@@ -1729,12 +1915,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -1749,11 +1941,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -2068,10 +2261,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A700F5A9-E5D3-4646-8DFA-7D1F89A425C9}">
-  <dimension ref="A1:AZ22"/>
+  <dimension ref="A1:BF22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="BA1" sqref="BA1:BD1"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2080,7 +2273,7 @@
     <col min="7" max="7" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:52" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:58" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B1" t="s">
         <v>21</v>
       </c>
@@ -2217,183 +2410,219 @@
         <v>98</v>
       </c>
       <c r="AU1" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="AV1" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="AW1" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="AX1" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="AY1" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="AZ1" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="2" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+        <v>105</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>129</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>130</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>131</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>132</v>
+      </c>
+      <c r="BE1" t="s">
+        <v>133</v>
+      </c>
+      <c r="BF1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" spans="1:58" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="2">
         <v>53.8</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="2">
         <v>63.5</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="2">
         <v>91.2</v>
       </c>
-      <c r="E2">
+      <c r="E2" s="2">
         <v>86.6</v>
       </c>
-      <c r="F2">
+      <c r="F2" s="2">
         <v>51.9</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="2">
         <v>45</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="2">
         <v>35.4</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="2">
         <v>4.4000000000000004</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="2">
         <v>4.7</v>
       </c>
-      <c r="K2">
+      <c r="K2" s="2">
         <v>21.5</v>
       </c>
-      <c r="L2">
+      <c r="L2" s="2">
         <v>34</v>
       </c>
-      <c r="M2">
+      <c r="M2" s="2">
         <v>21.8</v>
       </c>
-      <c r="N2">
+      <c r="N2" s="2">
         <v>9.1999999999999993</v>
       </c>
-      <c r="O2">
+      <c r="O2" s="2">
         <v>28.1</v>
       </c>
-      <c r="P2">
+      <c r="P2" s="2">
         <v>14.5</v>
       </c>
-      <c r="Q2">
+      <c r="Q2" s="2">
         <v>13.6</v>
       </c>
-      <c r="R2">
+      <c r="R2" s="2">
         <v>67</v>
       </c>
-      <c r="S2">
+      <c r="S2" s="2">
         <v>6.3</v>
       </c>
-      <c r="T2">
+      <c r="T2" s="2">
         <v>70</v>
       </c>
-      <c r="U2">
+      <c r="U2" s="2">
         <v>57.1</v>
       </c>
-      <c r="V2">
+      <c r="V2" s="2">
         <v>54.8</v>
       </c>
-      <c r="W2">
+      <c r="W2" s="2">
         <v>32</v>
       </c>
-      <c r="X2">
+      <c r="X2" s="2">
         <v>20.5</v>
       </c>
-      <c r="Y2">
+      <c r="Y2" s="2">
         <v>16.399999999999999</v>
       </c>
-      <c r="Z2">
+      <c r="Z2" s="2">
         <v>79.099999999999994</v>
       </c>
-      <c r="AA2">
+      <c r="AA2" s="2">
         <v>78.7</v>
       </c>
-      <c r="AB2">
+      <c r="AB2" s="2">
         <v>61.4</v>
       </c>
-      <c r="AC2">
+      <c r="AC2" s="2">
         <v>55.8</v>
       </c>
-      <c r="AD2">
+      <c r="AD2" s="2">
         <v>55.7</v>
       </c>
-      <c r="AE2">
+      <c r="AE2" s="2">
         <v>48.7</v>
       </c>
-      <c r="AF2">
+      <c r="AF2" s="2">
         <v>229</v>
       </c>
-      <c r="AG2">
+      <c r="AG2" s="2">
         <v>146</v>
       </c>
-      <c r="AH2">
+      <c r="AH2" s="2">
         <v>83</v>
       </c>
-      <c r="AI2">
+      <c r="AI2" s="2">
         <v>66.400000000000006</v>
       </c>
-      <c r="AJ2">
+      <c r="AJ2" s="2">
         <v>44.9</v>
       </c>
-      <c r="AK2">
+      <c r="AK2" s="2">
         <v>42.6</v>
       </c>
-      <c r="AL2">
+      <c r="AL2" s="2">
         <v>33.799999999999997</v>
       </c>
-      <c r="AM2">
+      <c r="AM2" s="2">
         <v>33.799999999999997</v>
       </c>
-      <c r="AN2">
+      <c r="AN2" s="2">
         <v>29</v>
       </c>
-      <c r="AO2">
+      <c r="AO2" s="2">
         <v>53.3</v>
       </c>
-      <c r="AP2">
+      <c r="AP2" s="2">
         <v>48.6</v>
       </c>
-      <c r="AQ2">
+      <c r="AQ2" s="2">
         <v>28.3</v>
       </c>
-      <c r="AR2">
+      <c r="AR2" s="2">
         <v>23.7</v>
       </c>
-      <c r="AS2">
+      <c r="AS2" s="2">
         <v>7.3</v>
       </c>
-      <c r="AT2">
+      <c r="AT2" s="2">
         <v>6.5</v>
       </c>
-      <c r="AU2">
+      <c r="AU2" s="2">
         <v>51.9</v>
       </c>
-      <c r="AV2">
+      <c r="AV2" s="2">
         <v>23.8</v>
       </c>
-      <c r="AW2">
+      <c r="AW2" s="2">
         <v>19.7</v>
       </c>
-      <c r="AX2">
+      <c r="AX2" s="2">
         <v>14</v>
       </c>
-      <c r="AY2">
+      <c r="AY2" s="2">
         <v>10.199999999999999</v>
       </c>
-      <c r="AZ2">
+      <c r="AZ2" s="2">
         <v>8.6</v>
       </c>
-    </row>
-    <row r="3" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA2" s="2">
+        <v>71.5</v>
+      </c>
+      <c r="BB2" s="2">
+        <v>64.599999999999994</v>
+      </c>
+      <c r="BC2" s="2">
+        <v>48.2</v>
+      </c>
+      <c r="BD2" s="2">
+        <v>44.4</v>
+      </c>
+      <c r="BE2" s="2">
+        <v>43.3</v>
+      </c>
+      <c r="BF2" s="2">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -2550,166 +2779,202 @@
       <c r="AZ3">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="BA3">
+        <v>63.6</v>
+      </c>
+      <c r="BB3">
+        <v>56.9</v>
+      </c>
+      <c r="BC3">
+        <v>37.9</v>
+      </c>
+      <c r="BD3">
+        <v>47.3</v>
+      </c>
+      <c r="BE3">
+        <v>27.3</v>
+      </c>
+      <c r="BF3">
+        <v>24.1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:58" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="2">
         <v>60.6</v>
       </c>
-      <c r="C4">
+      <c r="C4" s="2">
         <v>66.400000000000006</v>
       </c>
-      <c r="D4">
+      <c r="D4" s="2">
         <v>89.6</v>
       </c>
-      <c r="E4">
+      <c r="E4" s="2">
         <v>86</v>
       </c>
-      <c r="F4">
+      <c r="F4" s="2">
         <v>48.5</v>
       </c>
-      <c r="G4">
+      <c r="G4" s="2">
         <v>40.1</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="2">
         <v>31.5</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="2">
         <v>5</v>
       </c>
-      <c r="J4">
+      <c r="J4" s="2">
         <v>3.6</v>
       </c>
-      <c r="K4">
+      <c r="K4" s="2">
         <v>18.399999999999999</v>
       </c>
-      <c r="L4">
+      <c r="L4" s="2">
         <v>33.1</v>
       </c>
-      <c r="M4">
+      <c r="M4" s="2">
         <v>23.3</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="2">
         <v>11.2</v>
       </c>
-      <c r="O4">
+      <c r="O4" s="2">
         <v>29.1</v>
       </c>
-      <c r="P4">
+      <c r="P4" s="2">
         <v>16.600000000000001</v>
       </c>
-      <c r="Q4">
+      <c r="Q4" s="2">
         <v>12.5</v>
       </c>
-      <c r="R4">
+      <c r="R4" s="2">
         <v>66.400000000000006</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="2">
         <v>8.1999999999999993</v>
       </c>
-      <c r="T4">
+      <c r="T4" s="2">
         <v>67.3</v>
       </c>
-      <c r="U4">
+      <c r="U4" s="2">
         <v>58.1</v>
       </c>
-      <c r="V4">
+      <c r="V4" s="2">
         <v>57.2</v>
       </c>
-      <c r="W4">
+      <c r="W4" s="2">
         <v>31.2</v>
       </c>
-      <c r="X4">
+      <c r="X4" s="2">
         <v>29.2</v>
       </c>
-      <c r="Y4">
+      <c r="Y4" s="2">
         <v>19.3</v>
       </c>
-      <c r="Z4">
+      <c r="Z4" s="2">
         <v>73.400000000000006</v>
       </c>
-      <c r="AA4">
+      <c r="AA4" s="2">
         <v>79</v>
       </c>
-      <c r="AB4">
+      <c r="AB4" s="2">
         <v>61.5</v>
       </c>
-      <c r="AC4">
+      <c r="AC4" s="2">
         <v>61</v>
       </c>
-      <c r="AD4">
+      <c r="AD4" s="2">
         <v>58.7</v>
       </c>
-      <c r="AE4">
+      <c r="AE4" s="2">
         <v>56.2</v>
       </c>
-      <c r="AF4">
+      <c r="AF4" s="2">
         <v>253</v>
       </c>
-      <c r="AG4">
+      <c r="AG4" s="2">
         <v>168</v>
       </c>
-      <c r="AH4">
+      <c r="AH4" s="2">
         <v>85</v>
       </c>
-      <c r="AI4">
+      <c r="AI4" s="2">
         <v>68.2</v>
       </c>
-      <c r="AJ4">
+      <c r="AJ4" s="2">
         <v>45</v>
       </c>
-      <c r="AK4">
+      <c r="AK4" s="2">
         <v>44.2</v>
       </c>
-      <c r="AL4">
+      <c r="AL4" s="2">
         <v>41.6</v>
       </c>
-      <c r="AM4">
+      <c r="AM4" s="2">
         <v>42.3</v>
       </c>
-      <c r="AN4">
+      <c r="AN4" s="2">
         <v>32</v>
       </c>
-      <c r="AO4">
+      <c r="AO4" s="2">
         <v>60</v>
       </c>
-      <c r="AP4">
+      <c r="AP4" s="2">
         <v>54.1</v>
       </c>
-      <c r="AQ4">
+      <c r="AQ4" s="2">
         <v>36.1</v>
       </c>
-      <c r="AR4">
+      <c r="AR4" s="2">
         <v>30.9</v>
       </c>
-      <c r="AS4">
+      <c r="AS4" s="2">
         <v>9.5</v>
       </c>
-      <c r="AT4">
+      <c r="AT4" s="2">
         <v>8.1</v>
       </c>
-      <c r="AU4">
+      <c r="AU4" s="2">
         <v>48.5</v>
       </c>
-      <c r="AV4">
+      <c r="AV4" s="2">
         <v>28.5</v>
       </c>
-      <c r="AW4">
+      <c r="AW4" s="2">
         <v>21.8</v>
       </c>
-      <c r="AX4">
+      <c r="AX4" s="2">
         <v>16.100000000000001</v>
       </c>
-      <c r="AY4">
+      <c r="AY4" s="2">
         <v>11.9</v>
       </c>
-      <c r="AZ4">
+      <c r="AZ4" s="2">
         <v>11.1</v>
       </c>
-    </row>
-    <row r="5" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA4" s="2">
+        <v>71.7</v>
+      </c>
+      <c r="BB4" s="2">
+        <v>66.400000000000006</v>
+      </c>
+      <c r="BC4" s="2">
+        <v>48.6</v>
+      </c>
+      <c r="BD4" s="2">
+        <v>47.2</v>
+      </c>
+      <c r="BE4" s="2">
+        <v>40.5</v>
+      </c>
+      <c r="BF4" s="2">
+        <v>34.799999999999997</v>
+      </c>
+    </row>
+    <row r="5" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -2866,8 +3131,26 @@
       <c r="AZ5">
         <v>3.2</v>
       </c>
-    </row>
-    <row r="6" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA5">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="BB5">
+        <v>66.099999999999994</v>
+      </c>
+      <c r="BC5">
+        <v>47.8</v>
+      </c>
+      <c r="BD5">
+        <v>45.2</v>
+      </c>
+      <c r="BE5">
+        <v>34.6</v>
+      </c>
+      <c r="BF5">
+        <v>39.5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -3024,8 +3307,26 @@
       <c r="AZ6">
         <v>8.8000000000000007</v>
       </c>
-    </row>
-    <row r="7" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA6">
+        <v>83.3</v>
+      </c>
+      <c r="BB6">
+        <v>80</v>
+      </c>
+      <c r="BC6">
+        <v>59.2</v>
+      </c>
+      <c r="BD6">
+        <v>56.4</v>
+      </c>
+      <c r="BE6">
+        <v>42.9</v>
+      </c>
+      <c r="BF6">
+        <v>40.799999999999997</v>
+      </c>
+    </row>
+    <row r="7" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -3182,8 +3483,26 @@
       <c r="AZ7">
         <v>7.3</v>
       </c>
-    </row>
-    <row r="8" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA7">
+        <v>78.3</v>
+      </c>
+      <c r="BB7">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="BC7">
+        <v>58</v>
+      </c>
+      <c r="BD7">
+        <v>52.1</v>
+      </c>
+      <c r="BE7">
+        <v>50.3</v>
+      </c>
+      <c r="BF7">
+        <v>41.1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -3340,8 +3659,26 @@
       <c r="AZ8">
         <v>4.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA8">
+        <v>69.599999999999994</v>
+      </c>
+      <c r="BB8">
+        <v>60.4</v>
+      </c>
+      <c r="BC8">
+        <v>41.8</v>
+      </c>
+      <c r="BD8">
+        <v>51.4</v>
+      </c>
+      <c r="BE8">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="BF8">
+        <v>28.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -3498,8 +3835,26 @@
       <c r="AZ9">
         <v>3.3</v>
       </c>
-    </row>
-    <row r="10" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA9">
+        <v>67.2</v>
+      </c>
+      <c r="BB9">
+        <v>62.6</v>
+      </c>
+      <c r="BC9">
+        <v>40.1</v>
+      </c>
+      <c r="BD9">
+        <v>45.4</v>
+      </c>
+      <c r="BE9">
+        <v>28.2</v>
+      </c>
+      <c r="BF9">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -3656,8 +4011,26 @@
       <c r="AZ10">
         <v>19.8</v>
       </c>
-    </row>
-    <row r="11" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA10">
+        <v>72.599999999999994</v>
+      </c>
+      <c r="BB10">
+        <v>68.2</v>
+      </c>
+      <c r="BC10">
+        <v>53.1</v>
+      </c>
+      <c r="BD10">
+        <v>49.4</v>
+      </c>
+      <c r="BE10">
+        <v>46.2</v>
+      </c>
+      <c r="BF10">
+        <v>38.200000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -3814,8 +4187,26 @@
       <c r="AZ11">
         <v>12.4</v>
       </c>
-    </row>
-    <row r="12" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA11">
+        <v>67.5</v>
+      </c>
+      <c r="BB11">
+        <v>63.4</v>
+      </c>
+      <c r="BC11">
+        <v>45.4</v>
+      </c>
+      <c r="BD11">
+        <v>40.299999999999997</v>
+      </c>
+      <c r="BE11">
+        <v>37.6</v>
+      </c>
+      <c r="BF11">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -3972,8 +4363,26 @@
       <c r="AZ12">
         <v>9.8000000000000007</v>
       </c>
-    </row>
-    <row r="13" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA12">
+        <v>70.8</v>
+      </c>
+      <c r="BB12">
+        <v>65.900000000000006</v>
+      </c>
+      <c r="BC12">
+        <v>50.4</v>
+      </c>
+      <c r="BD12">
+        <v>43</v>
+      </c>
+      <c r="BE12">
+        <v>42.4</v>
+      </c>
+      <c r="BF12">
+        <v>27.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -4130,8 +4539,26 @@
       <c r="AZ13">
         <v>14.6</v>
       </c>
-    </row>
-    <row r="14" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA13">
+        <v>76.8</v>
+      </c>
+      <c r="BB13">
+        <v>71.400000000000006</v>
+      </c>
+      <c r="BC13">
+        <v>50.3</v>
+      </c>
+      <c r="BD13">
+        <v>48.9</v>
+      </c>
+      <c r="BE13">
+        <v>42.3</v>
+      </c>
+      <c r="BF13">
+        <v>41.2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -4288,8 +4715,26 @@
       <c r="AZ14">
         <v>3.9</v>
       </c>
-    </row>
-    <row r="15" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA14">
+        <v>64.400000000000006</v>
+      </c>
+      <c r="BB14">
+        <v>56.2</v>
+      </c>
+      <c r="BC14">
+        <v>36.299999999999997</v>
+      </c>
+      <c r="BD14">
+        <v>43.1</v>
+      </c>
+      <c r="BE14">
+        <v>30.1</v>
+      </c>
+      <c r="BF14">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="15" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -4446,8 +4891,26 @@
       <c r="AZ15">
         <v>4.3</v>
       </c>
-    </row>
-    <row r="16" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA15">
+        <v>69.400000000000006</v>
+      </c>
+      <c r="BB15">
+        <v>61.8</v>
+      </c>
+      <c r="BC15">
+        <v>43.4</v>
+      </c>
+      <c r="BD15">
+        <v>44.4</v>
+      </c>
+      <c r="BE15">
+        <v>38.799999999999997</v>
+      </c>
+      <c r="BF15">
+        <v>32.299999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -4604,8 +5067,26 @@
       <c r="AZ16">
         <v>4</v>
       </c>
-    </row>
-    <row r="17" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA16">
+        <v>65.2</v>
+      </c>
+      <c r="BB16">
+        <v>59.1</v>
+      </c>
+      <c r="BC16">
+        <v>42.7</v>
+      </c>
+      <c r="BD16">
+        <v>42.7</v>
+      </c>
+      <c r="BE16">
+        <v>38</v>
+      </c>
+      <c r="BF16">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -4762,166 +5243,202 @@
       <c r="AZ17">
         <v>11.6</v>
       </c>
-    </row>
-    <row r="18" spans="1:52" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
+      <c r="BA17">
+        <v>79.900000000000006</v>
+      </c>
+      <c r="BB17">
+        <v>61.5</v>
+      </c>
+      <c r="BC17">
+        <v>37.9</v>
+      </c>
+      <c r="BD17">
+        <v>33.9</v>
+      </c>
+      <c r="BE17">
+        <v>30.3</v>
+      </c>
+      <c r="BF17">
+        <v>49.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:58" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="2">
         <v>43.2</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="2">
         <v>55.4</v>
       </c>
-      <c r="D18">
+      <c r="D18" s="2">
         <v>91.3</v>
       </c>
-      <c r="E18">
+      <c r="E18" s="2">
         <v>85.3</v>
       </c>
-      <c r="F18">
+      <c r="F18" s="2">
         <v>63.4</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="2">
         <v>47</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="2">
         <v>38.799999999999997</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="2">
         <v>2.2000000000000002</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="2">
         <v>6</v>
       </c>
-      <c r="K18">
+      <c r="K18" s="2">
         <v>24.4</v>
       </c>
-      <c r="L18">
+      <c r="L18" s="2">
         <v>33.700000000000003</v>
       </c>
-      <c r="M18">
+      <c r="M18" s="2">
         <v>20.5</v>
       </c>
-      <c r="N18">
+      <c r="N18" s="2">
         <v>6.7</v>
       </c>
-      <c r="O18">
+      <c r="O18" s="2">
         <v>27</v>
       </c>
-      <c r="P18">
+      <c r="P18" s="2">
         <v>10.7</v>
       </c>
-      <c r="Q18">
+      <c r="Q18" s="2">
         <v>16.3</v>
       </c>
-      <c r="R18">
+      <c r="R18" s="2">
         <v>65</v>
       </c>
-      <c r="S18">
+      <c r="S18" s="2">
         <v>4.2</v>
       </c>
-      <c r="T18">
+      <c r="T18" s="2">
         <v>67.2</v>
       </c>
-      <c r="U18">
+      <c r="U18" s="2">
         <v>53.1</v>
       </c>
-      <c r="V18">
+      <c r="V18" s="2">
         <v>47.5</v>
       </c>
-      <c r="W18">
+      <c r="W18" s="2">
         <v>30.4</v>
       </c>
-      <c r="X18">
+      <c r="X18" s="2">
         <v>6.8</v>
       </c>
-      <c r="Y18">
+      <c r="Y18" s="2">
         <v>11.6</v>
       </c>
-      <c r="Z18">
+      <c r="Z18" s="2">
         <v>83.7</v>
       </c>
-      <c r="AA18">
+      <c r="AA18" s="2">
         <v>74.3</v>
       </c>
-      <c r="AB18">
+      <c r="AB18" s="2">
         <v>57.4</v>
       </c>
-      <c r="AC18">
+      <c r="AC18" s="2">
         <v>45.9</v>
       </c>
-      <c r="AD18">
+      <c r="AD18" s="2">
         <v>45.5</v>
       </c>
-      <c r="AE18">
+      <c r="AE18" s="2">
         <v>35.5</v>
       </c>
-      <c r="AF18">
+      <c r="AF18" s="2">
         <v>123</v>
       </c>
-      <c r="AG18">
+      <c r="AG18" s="2">
         <v>63</v>
       </c>
-      <c r="AH18">
+      <c r="AH18" s="2">
         <v>60</v>
       </c>
-      <c r="AI18">
+      <c r="AI18" s="2">
         <v>61.1</v>
       </c>
-      <c r="AJ18">
+      <c r="AJ18" s="2">
         <v>45.5</v>
       </c>
-      <c r="AK18">
+      <c r="AK18" s="2">
         <v>35.6</v>
       </c>
-      <c r="AL18">
+      <c r="AL18" s="2">
         <v>24</v>
       </c>
-      <c r="AM18">
+      <c r="AM18" s="2">
         <v>19</v>
       </c>
-      <c r="AN18">
+      <c r="AN18" s="2">
         <v>25.8</v>
       </c>
-      <c r="AO18">
+      <c r="AO18" s="2">
         <v>54.6</v>
       </c>
-      <c r="AP18">
+      <c r="AP18" s="2">
         <v>52.1</v>
       </c>
-      <c r="AQ18">
+      <c r="AQ18" s="2">
         <v>19.600000000000001</v>
       </c>
-      <c r="AR18">
+      <c r="AR18" s="2">
         <v>16.3</v>
       </c>
-      <c r="AS18">
+      <c r="AS18" s="2">
         <v>3.3</v>
       </c>
-      <c r="AT18">
+      <c r="AT18" s="2">
         <v>4.5</v>
       </c>
-      <c r="AU18">
+      <c r="AU18" s="2">
         <v>63.4</v>
       </c>
-      <c r="AV18">
+      <c r="AV18" s="2">
         <v>31.9</v>
       </c>
-      <c r="AW18">
+      <c r="AW18" s="2">
         <v>20.9</v>
       </c>
-      <c r="AX18">
+      <c r="AX18" s="2">
         <v>15.1</v>
       </c>
-      <c r="AY18">
+      <c r="AY18" s="2">
         <v>8.3000000000000007</v>
       </c>
-      <c r="AZ18">
+      <c r="AZ18" s="2">
         <v>6.7</v>
       </c>
-    </row>
-    <row r="19" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA18" s="2">
+        <v>71.900000000000006</v>
+      </c>
+      <c r="BB18" s="2">
+        <v>66.3</v>
+      </c>
+      <c r="BC18" s="2">
+        <v>52.9</v>
+      </c>
+      <c r="BD18" s="2">
+        <v>44.2</v>
+      </c>
+      <c r="BE18" s="2">
+        <v>49.7</v>
+      </c>
+      <c r="BF18" s="2">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="19" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -5078,8 +5595,26 @@
       <c r="AZ19">
         <v>8.5</v>
       </c>
-    </row>
-    <row r="20" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA19">
+        <v>82.5</v>
+      </c>
+      <c r="BB19">
+        <v>76.599999999999994</v>
+      </c>
+      <c r="BC19">
+        <v>57.4</v>
+      </c>
+      <c r="BD19">
+        <v>55.3</v>
+      </c>
+      <c r="BE19">
+        <v>53</v>
+      </c>
+      <c r="BF19">
+        <v>54.2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -5236,8 +5771,26 @@
       <c r="AZ20">
         <v>9.1</v>
       </c>
-    </row>
-    <row r="21" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA20">
+        <v>87.3</v>
+      </c>
+      <c r="BB20">
+        <v>82.9</v>
+      </c>
+      <c r="BC20">
+        <v>73.400000000000006</v>
+      </c>
+      <c r="BD20">
+        <v>63.8</v>
+      </c>
+      <c r="BE20">
+        <v>71.7</v>
+      </c>
+      <c r="BF20">
+        <v>42.5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -5394,8 +5947,26 @@
       <c r="AZ21">
         <v>4.9000000000000004</v>
       </c>
-    </row>
-    <row r="22" spans="1:52" x14ac:dyDescent="0.3">
+      <c r="BA21">
+        <v>60.3</v>
+      </c>
+      <c r="BB21">
+        <v>54</v>
+      </c>
+      <c r="BC21">
+        <v>38.299999999999997</v>
+      </c>
+      <c r="BD21">
+        <v>29.6</v>
+      </c>
+      <c r="BE21">
+        <v>34.200000000000003</v>
+      </c>
+      <c r="BF21">
+        <v>18.7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:58" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -5551,6 +6122,24 @@
       </c>
       <c r="AZ22">
         <v>3.5</v>
+      </c>
+      <c r="BA22">
+        <v>69.099999999999994</v>
+      </c>
+      <c r="BB22">
+        <v>59.5</v>
+      </c>
+      <c r="BC22">
+        <v>46.9</v>
+      </c>
+      <c r="BD22">
+        <v>38.5</v>
+      </c>
+      <c r="BE22">
+        <v>50.1</v>
+      </c>
+      <c r="BF22">
+        <v>25.3</v>
       </c>
     </row>
   </sheetData>
@@ -5560,10 +6149,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB330550-DD18-498F-81BC-F9C6406C0566}">
-  <dimension ref="A1:A51"/>
+  <dimension ref="A1:A57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -5763,67 +6352,97 @@
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>104</v>
+        <v>116</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>107</v>
+        <v>119</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>109</v>
+        <v>121</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
     </row>
     <row r="49" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>122</v>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>128</v>
       </c>
     </row>
   </sheetData>

</xml_diff>